<commit_message>
Update swimming app keywords database
</commit_message>
<xml_diff>
--- a/data_mining/swimming app.xlsx
+++ b/data_mining/swimming app.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/user/Desktop/研究計畫/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{726C4AFD-15A8-C248-BDF0-794969989A24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C9988B8-0F78-A348-AA39-B56B265191A9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16280" xr2:uid="{11AA6ECC-5B8B-674D-9AF5-226EDF27D115}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{11AA6ECC-5B8B-674D-9AF5-226EDF27D115}"/>
   </bookViews>
   <sheets>
     <sheet name="app分析" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="40">
   <si>
     <t>Duoswim:swim workout app</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -190,6 +190,52 @@
   </si>
   <si>
     <t>no data</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>garmin connect</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>整體使用上都很不錯記錄游泳功能很常出錯（4440）</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>記錄距離
+設定泳池大小
+泳姿辨識
+自動休息
+技術訓練日誌</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>EN/CH</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FREE(garmin watch)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>無法同步(122)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>free(apple watch)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>fitness</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>automatically tracks your splits and auto sets
+view the type of strokes you performed during your swim
+workout time
+calories
+heart rate
+avg pace
+laps</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -259,7 +305,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -279,6 +325,9 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -595,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA813BCC-FC93-B641-A691-3954FC49A367}">
-  <dimension ref="A1:F7"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="84" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -609,10 +658,11 @@
     <col min="4" max="4" width="32" customWidth="1"/>
     <col min="5" max="5" width="78" customWidth="1"/>
     <col min="6" max="6" width="60.5" customWidth="1"/>
-    <col min="7" max="7" width="57" customWidth="1"/>
+    <col min="7" max="7" width="25" customWidth="1"/>
+    <col min="8" max="8" width="59.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22">
+    <row r="1" spans="1:8" ht="22">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -628,8 +678,14 @@
       <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="G1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" ht="32">
+    <row r="2" spans="1:8" ht="32">
       <c r="A2" s="2" t="s">
         <v>29</v>
       </c>
@@ -648,8 +704,14 @@
       <c r="F2" t="s">
         <v>15</v>
       </c>
+      <c r="G2" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" t="s">
+        <v>36</v>
+      </c>
     </row>
-    <row r="3" spans="1:6" ht="22">
+    <row r="3" spans="1:8" ht="22">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -668,8 +730,14 @@
       <c r="F3" t="s">
         <v>30</v>
       </c>
+      <c r="G3" s="7">
+        <v>2014</v>
+      </c>
+      <c r="H3" s="7">
+        <v>2011</v>
+      </c>
     </row>
-    <row r="4" spans="1:6" ht="48">
+    <row r="4" spans="1:8" ht="48">
       <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
@@ -688,8 +756,14 @@
       <c r="F4" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="G4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>37</v>
+      </c>
     </row>
-    <row r="5" spans="1:6" ht="288">
+    <row r="5" spans="1:8" ht="288">
       <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
@@ -708,8 +782,14 @@
       <c r="F5" s="4" t="s">
         <v>23</v>
       </c>
+      <c r="G5" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>39</v>
+      </c>
     </row>
-    <row r="6" spans="1:6" ht="45" customHeight="1">
+    <row r="6" spans="1:8" ht="45" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -728,8 +808,14 @@
       <c r="F6" t="s">
         <v>10</v>
       </c>
+      <c r="G6" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" t="s">
+        <v>34</v>
+      </c>
     </row>
-    <row r="7" spans="1:6" ht="22">
+    <row r="7" spans="1:8" ht="22">
       <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
@@ -743,6 +829,9 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>